<commit_message>
Update US001 - Quality Assurance Checklist Create Client v1.xlsx
</commit_message>
<xml_diff>
--- a/US001 - Quality Assurance Checklist Create Client v1.xlsx
+++ b/US001 - Quality Assurance Checklist Create Client v1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\haing\Download\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\haing\Download\demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{596C9D34-05F7-437E-8A9D-35BE9275B813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3740CFA4-8120-41B2-844D-B13CA02A2BC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="4" r:id="rId1"/>
@@ -148,7 +148,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="100">
   <si>
     <t>Quality Assurance Checklist</t>
   </si>
@@ -162,19 +162,10 @@
     <t>Fresher</t>
   </si>
   <si>
-    <t>Nguyen Ngoc Bao Trong</t>
-  </si>
-  <si>
     <t>Mentor</t>
   </si>
   <si>
-    <t>Nguyen Ba Qui</t>
-  </si>
-  <si>
     <t>GIT</t>
-  </si>
-  <si>
-    <t>https://github.dxc.com/tnguyen704/US001</t>
   </si>
   <si>
     <t>Online</t>
@@ -314,144 +305,21 @@
     <t>Remarks</t>
   </si>
   <si>
-    <t>Client</t>
-  </si>
-  <si>
     <t>Java</t>
   </si>
   <si>
     <t>Add</t>
   </si>
   <si>
-    <t>Trong Nguyen</t>
-  </si>
-  <si>
-    <t>https://github.dxc.com/tnguyen704/US001/blob/main/US001_BE/src/main/java/com/dxc/technology/model/Client.java</t>
-  </si>
-  <si>
-    <t>ClientRepository</t>
-  </si>
-  <si>
-    <t>https://github.dxc.com/tnguyen704/US001/blob/main/US001_BE/src/main/java/com/dxc/technology/repository/ClientRepository.java</t>
-  </si>
-  <si>
-    <t>ClientService</t>
-  </si>
-  <si>
-    <t>https://github.dxc.com/tnguyen704/US001/blob/main/US001_BE/src/main/java/com/dxc/technology/service/ClientService.java</t>
-  </si>
-  <si>
-    <t>ClientServiceImpl</t>
-  </si>
-  <si>
-    <t>https://github.dxc.com/tnguyen704/US001/blob/main/US001_BE/src/main/java/com/dxc/technology/serviceImpl/ClientServiceImpl.java</t>
-  </si>
-  <si>
-    <t>ClientController</t>
-  </si>
-  <si>
-    <t>https://github.dxc.com/tnguyen704/US001/blob/main/US001_BE/src/main/java/com/dxc/technology/controller/ClientController.java</t>
-  </si>
-  <si>
-    <t>ClientWebController</t>
-  </si>
-  <si>
-    <t>https://github.dxc.com/tnguyen704/US001/blob/main/US001_BE/src/main/java/com/dxc/technology/controller/ClientWebController.java</t>
-  </si>
-  <si>
     <t>Configuration</t>
   </si>
   <si>
-    <t>Internationalization</t>
-  </si>
-  <si>
-    <t>https://github.dxc.com/tnguyen704/US001/blob/main/US001_BE/src/main/java/com/dxc/technology/configs/Internationalization.java</t>
-  </si>
-  <si>
-    <t>ClientNotFoundException</t>
-  </si>
-  <si>
-    <t>https://github.dxc.com/tnguyen704/US001/blob/main/US001_BE/src/main/java/com/dxc/technology/exceptions/ClientNotFoundException.java</t>
-  </si>
-  <si>
-    <t>ClientNotFoundResponse</t>
-  </si>
-  <si>
-    <t>https://github.dxc.com/tnguyen704/US001/blob/main/US001_BE/src/main/java/com/dxc/technology/exceptions/ClientNotFoundResponse.java</t>
-  </si>
-  <si>
-    <t>MessageException</t>
-  </si>
-  <si>
-    <t>https://github.dxc.com/tnguyen704/US001/blob/main/US001_BE/src/main/java/com/dxc/technology/exceptions/MessageException.java</t>
-  </si>
-  <si>
-    <t>ClientDTO</t>
-  </si>
-  <si>
-    <t>https://github.dxc.com/tnguyen704/US001/blob/main/US001_BE/src/main/java/com/dxc/technology/dto/ClientDTO.java</t>
-  </si>
-  <si>
-    <t>Us001BeApplication</t>
-  </si>
-  <si>
-    <t>https://github.dxc.com/tnguyen704/US001/blob/main/US001_BE/src/test/java/com/dxc/technology/Us001BeApplicationTests.java</t>
-  </si>
-  <si>
-    <t>details_client</t>
-  </si>
-  <si>
     <t>Others</t>
   </si>
   <si>
-    <t>https://github.dxc.com/tnguyen704/US001/blob/main/US001_BE/src/main/resources/templates/details_client.html</t>
-  </si>
-  <si>
-    <t>list_clients</t>
-  </si>
-  <si>
-    <t>https://github.dxc.com/tnguyen704/US001/blob/main/US001_BE/src/main/resources/templates/list_clients.html</t>
-  </si>
-  <si>
-    <t>modify_client</t>
-  </si>
-  <si>
-    <t>https://github.dxc.com/tnguyen704/US001/blob/main/US001_BE/src/main/resources/templates/modify_client.html</t>
-  </si>
-  <si>
-    <t>new_client</t>
-  </si>
-  <si>
-    <t>https://github.dxc.com/tnguyen704/US001/blob/main/US001_BE/src/main/resources/templates/new_client.html</t>
-  </si>
-  <si>
-    <t>application</t>
-  </si>
-  <si>
     <t>Properties</t>
   </si>
   <si>
-    <t>https://github.dxc.com/tnguyen704/US001/blob/main/US001_BE/src/main/resources/application.properties</t>
-  </si>
-  <si>
-    <t>log4j</t>
-  </si>
-  <si>
-    <t>https://github.dxc.com/tnguyen704/US001/blob/main/US001_BE/src/main/resources/log4j.properties</t>
-  </si>
-  <si>
-    <t>messages</t>
-  </si>
-  <si>
-    <t>https://github.dxc.com/tnguyen704/US001/blob/main/US001_BE/src/main/resources/messages.properties</t>
-  </si>
-  <si>
-    <t>message_vi</t>
-  </si>
-  <si>
-    <t>https://github.dxc.com/tnguyen704/US001/blob/main/US001_BE/src/main/resources/messages_vi.properties</t>
-  </si>
-  <si>
     <t>Action</t>
   </si>
   <si>
@@ -573,6 +441,15 @@
   </si>
   <si>
     <t>No Completed</t>
+  </si>
+  <si>
+    <t>Nguyen Ngoc Hai</t>
+  </si>
+  <si>
+    <t>Dang Danh Huu</t>
+  </si>
+  <si>
+    <t>https://github.com/hai0626/DemoClient</t>
   </si>
 </sst>
 </file>
@@ -1508,7 +1385,7 @@
   <dimension ref="C4:G19"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1540,23 +1417,23 @@
         <v>3</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C9" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>6</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="3:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C10" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E10" s="37" t="s">
-        <v>8</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="3:7" x14ac:dyDescent="0.25">
@@ -1569,46 +1446,46 @@
     </row>
     <row r="13" spans="3:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="E13" s="28" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F13" s="28" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G13" s="28" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C14" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E14" s="21" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F14" s="21" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G14" s="21" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E15" s="21" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F15" s="21"/>
       <c r="G15" s="21"/>
     </row>
     <row r="16" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E16" s="21" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F16" s="21"/>
       <c r="G16" s="21"/>
     </row>
     <row r="17" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E17" s="21" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F17" s="21"/>
       <c r="G17" s="21"/>
@@ -1643,7 +1520,7 @@
   </sheetPr>
   <dimension ref="A2:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -1658,16 +1535,16 @@
   <sheetData>
     <row r="2" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="18" t="s">
         <v>18</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1675,13 +1552,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="36" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C3" s="60" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
@@ -1689,13 +1566,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C4" s="61" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D4" s="35" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
@@ -1703,13 +1580,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="53" t="s">
-        <v>124</v>
+        <v>80</v>
       </c>
       <c r="C5" s="61" t="s">
-        <v>125</v>
+        <v>81</v>
       </c>
       <c r="D5" s="35" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -1717,13 +1594,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="54" t="s">
-        <v>126</v>
+        <v>82</v>
       </c>
       <c r="C6" s="57" t="s">
-        <v>133</v>
+        <v>89</v>
       </c>
       <c r="D6" s="35" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
@@ -1731,13 +1608,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="55" t="s">
-        <v>127</v>
+        <v>83</v>
       </c>
       <c r="C7" s="58" t="s">
-        <v>134</v>
+        <v>90</v>
       </c>
       <c r="D7" s="35" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -1745,13 +1622,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="55" t="s">
-        <v>128</v>
+        <v>84</v>
       </c>
       <c r="C8" s="58" t="s">
-        <v>135</v>
+        <v>91</v>
       </c>
       <c r="D8" s="35" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -1759,13 +1636,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="55" t="s">
-        <v>129</v>
+        <v>85</v>
       </c>
       <c r="C9" s="58" t="s">
-        <v>136</v>
+        <v>92</v>
       </c>
       <c r="D9" s="35" t="s">
-        <v>140</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -1773,13 +1650,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="55" t="s">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="C10" s="58" t="s">
-        <v>137</v>
+        <v>93</v>
       </c>
       <c r="D10" s="35" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
@@ -1787,13 +1664,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="55" t="s">
-        <v>131</v>
+        <v>87</v>
       </c>
       <c r="C11" s="58" t="s">
-        <v>138</v>
+        <v>94</v>
       </c>
       <c r="D11" s="35" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
@@ -1801,13 +1678,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="56" t="s">
-        <v>132</v>
+        <v>88</v>
       </c>
       <c r="C12" s="59" t="s">
-        <v>139</v>
+        <v>95</v>
       </c>
       <c r="D12" s="35" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1839,16 +1716,16 @@
   <sheetData>
     <row r="2" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="18" t="s">
         <v>18</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1856,13 +1733,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="36" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C3" s="60" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
@@ -1870,13 +1747,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C4" s="61" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1884,13 +1761,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C5" s="62" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1898,13 +1775,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C6" s="63" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1912,13 +1789,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="36" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C7" s="62" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1926,13 +1803,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="36" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C8" s="63" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1963,16 +1840,16 @@
   <sheetData>
     <row r="2" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="18" t="s">
         <v>18</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1980,13 +1857,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="36" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C3" s="60" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
@@ -1994,13 +1871,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C4" s="61" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
@@ -2008,13 +1885,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C5" s="64" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2039,8 +1916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2059,578 +1936,258 @@
   <sheetData>
     <row r="1" spans="1:9" ht="22.8" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="23"/>
     </row>
     <row r="2" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="44" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B2" s="44" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="44" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="F2" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="G2" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="44" t="s">
+      <c r="H2" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="44" t="s">
+      <c r="I2" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="44" t="s">
-        <v>51</v>
-      </c>
-      <c r="H2" s="44" t="s">
-        <v>52</v>
-      </c>
-      <c r="I2" s="44" t="s">
-        <v>53</v>
-      </c>
     </row>
     <row r="3" spans="1:9" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="52">
-        <v>1</v>
-      </c>
-      <c r="B3" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="D3" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="E3" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="F3" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="G3" s="46">
-        <v>44782</v>
-      </c>
-      <c r="H3" s="50" t="s">
-        <v>58</v>
-      </c>
+      <c r="A3" s="52"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="50"/>
       <c r="I3" s="41"/>
     </row>
-    <row r="4" spans="1:9" ht="57.6" x14ac:dyDescent="0.25">
-      <c r="A4" s="43">
-        <v>2</v>
-      </c>
-      <c r="B4" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="49" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="E4" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="F4" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="G4" s="46">
-        <v>44782</v>
-      </c>
-      <c r="H4" s="48" t="s">
-        <v>60</v>
-      </c>
+    <row r="4" spans="1:9" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A4" s="43"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="48"/>
       <c r="I4" s="42"/>
     </row>
-    <row r="5" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="52">
-        <v>3</v>
-      </c>
-      <c r="B5" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="49" t="s">
-        <v>61</v>
-      </c>
-      <c r="D5" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="E5" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="F5" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="G5" s="46">
-        <v>44782</v>
-      </c>
-      <c r="H5" s="51" t="s">
-        <v>62</v>
-      </c>
+    <row r="5" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="52"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="51"/>
       <c r="I5" s="42"/>
     </row>
-    <row r="6" spans="1:9" ht="57.6" x14ac:dyDescent="0.25">
-      <c r="A6" s="43">
-        <v>4</v>
-      </c>
-      <c r="B6" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="49" t="s">
-        <v>63</v>
-      </c>
-      <c r="D6" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="E6" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="F6" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="G6" s="46">
-        <v>44782</v>
-      </c>
-      <c r="H6" s="48" t="s">
-        <v>64</v>
-      </c>
+    <row r="6" spans="1:9" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A6" s="43"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="48"/>
       <c r="I6" s="42"/>
     </row>
-    <row r="7" spans="1:9" ht="57.6" x14ac:dyDescent="0.25">
-      <c r="A7" s="52">
-        <v>5</v>
-      </c>
-      <c r="B7" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="49" t="s">
-        <v>65</v>
-      </c>
-      <c r="D7" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="E7" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="F7" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="G7" s="46">
-        <v>44782</v>
-      </c>
-      <c r="H7" s="48" t="s">
-        <v>66</v>
-      </c>
+    <row r="7" spans="1:9" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A7" s="52"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="48"/>
       <c r="I7" s="42"/>
     </row>
-    <row r="8" spans="1:9" ht="57.6" x14ac:dyDescent="0.25">
-      <c r="A8" s="43">
-        <v>6</v>
-      </c>
-      <c r="B8" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="D8" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="E8" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="F8" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="G8" s="46">
-        <v>44783</v>
-      </c>
-      <c r="H8" s="48" t="s">
-        <v>68</v>
-      </c>
+    <row r="8" spans="1:9" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A8" s="43"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="48"/>
       <c r="I8" s="42"/>
     </row>
-    <row r="9" spans="1:9" ht="57.6" x14ac:dyDescent="0.25">
-      <c r="A9" s="52">
-        <v>7</v>
-      </c>
-      <c r="B9" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="C9" s="49" t="s">
-        <v>70</v>
-      </c>
-      <c r="D9" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="E9" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="F9" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="G9" s="45">
-        <v>44785</v>
-      </c>
-      <c r="H9" s="48" t="s">
-        <v>71</v>
-      </c>
+    <row r="9" spans="1:9" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A9" s="52"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="48"/>
       <c r="I9" s="42"/>
     </row>
-    <row r="10" spans="1:9" ht="57.6" x14ac:dyDescent="0.25">
-      <c r="A10" s="43">
-        <v>8</v>
-      </c>
-      <c r="B10" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="49" t="s">
-        <v>72</v>
-      </c>
-      <c r="D10" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="E10" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="F10" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="G10" s="45">
-        <v>44783</v>
-      </c>
-      <c r="H10" s="48" t="s">
-        <v>73</v>
-      </c>
+    <row r="10" spans="1:9" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A10" s="43"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="48"/>
       <c r="I10" s="42"/>
     </row>
-    <row r="11" spans="1:9" ht="57.6" x14ac:dyDescent="0.25">
-      <c r="A11" s="52">
-        <v>9</v>
-      </c>
-      <c r="B11" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="49" t="s">
-        <v>74</v>
-      </c>
-      <c r="D11" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="E11" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="F11" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="G11" s="45">
-        <v>44783</v>
-      </c>
-      <c r="H11" s="48" t="s">
-        <v>75</v>
-      </c>
+    <row r="11" spans="1:9" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A11" s="52"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="48"/>
       <c r="I11" s="42"/>
     </row>
     <row r="12" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="43">
-        <v>10</v>
-      </c>
-      <c r="B12" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="49" t="s">
-        <v>76</v>
-      </c>
-      <c r="D12" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="E12" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="F12" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="G12" s="45">
-        <v>44785</v>
-      </c>
-      <c r="H12" s="48" t="s">
-        <v>77</v>
-      </c>
+      <c r="A12" s="43"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="45"/>
+      <c r="H12" s="48"/>
       <c r="I12" s="42"/>
     </row>
-    <row r="13" spans="1:9" ht="43.2" x14ac:dyDescent="0.25">
-      <c r="A13" s="52">
-        <v>11</v>
-      </c>
-      <c r="B13" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="49" t="s">
-        <v>78</v>
-      </c>
-      <c r="D13" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="E13" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="F13" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="G13" s="45">
-        <v>44785</v>
-      </c>
-      <c r="H13" s="48" t="s">
-        <v>79</v>
-      </c>
+    <row r="13" spans="1:9" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A13" s="52"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="48"/>
       <c r="I13" s="42"/>
     </row>
-    <row r="14" spans="1:9" ht="57.6" x14ac:dyDescent="0.25">
-      <c r="A14" s="43">
-        <v>12</v>
-      </c>
-      <c r="B14" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="49" t="s">
-        <v>80</v>
-      </c>
-      <c r="D14" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="E14" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="F14" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="G14" s="45">
-        <v>44782</v>
-      </c>
-      <c r="H14" s="48" t="s">
-        <v>81</v>
-      </c>
+    <row r="14" spans="1:9" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A14" s="43"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="49"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="48"/>
       <c r="I14" s="42"/>
     </row>
-    <row r="15" spans="1:9" ht="43.2" x14ac:dyDescent="0.25">
-      <c r="A15" s="52">
-        <v>13</v>
-      </c>
-      <c r="B15" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="49" t="s">
-        <v>82</v>
-      </c>
-      <c r="D15" s="40" t="s">
-        <v>83</v>
-      </c>
-      <c r="E15" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="F15" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="G15" s="45">
-        <v>44784</v>
-      </c>
-      <c r="H15" s="48" t="s">
-        <v>84</v>
-      </c>
+    <row r="15" spans="1:9" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A15" s="52"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="48"/>
       <c r="I15" s="42"/>
     </row>
-    <row r="16" spans="1:9" ht="43.2" x14ac:dyDescent="0.25">
-      <c r="A16" s="43">
-        <v>14</v>
-      </c>
-      <c r="B16" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="49" t="s">
-        <v>85</v>
-      </c>
-      <c r="D16" s="40" t="s">
-        <v>83</v>
-      </c>
-      <c r="E16" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="F16" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="G16" s="45">
-        <v>44783</v>
-      </c>
-      <c r="H16" s="48" t="s">
-        <v>86</v>
-      </c>
+    <row r="16" spans="1:9" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A16" s="43"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="49"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="48"/>
       <c r="I16" s="42"/>
     </row>
-    <row r="17" spans="1:9" ht="43.2" x14ac:dyDescent="0.25">
-      <c r="A17" s="52">
-        <v>15</v>
-      </c>
-      <c r="B17" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="49" t="s">
-        <v>87</v>
-      </c>
-      <c r="D17" s="40" t="s">
-        <v>83</v>
-      </c>
-      <c r="E17" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="F17" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="G17" s="45">
-        <v>44784</v>
-      </c>
-      <c r="H17" s="48" t="s">
-        <v>88</v>
-      </c>
+    <row r="17" spans="1:9" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A17" s="52"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="48"/>
       <c r="I17" s="42"/>
     </row>
-    <row r="18" spans="1:9" ht="43.2" x14ac:dyDescent="0.25">
-      <c r="A18" s="43">
-        <v>16</v>
-      </c>
-      <c r="B18" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="49" t="s">
-        <v>89</v>
-      </c>
-      <c r="D18" s="40" t="s">
-        <v>83</v>
-      </c>
-      <c r="E18" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="F18" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="G18" s="45">
-        <v>44784</v>
-      </c>
-      <c r="H18" s="48" t="s">
-        <v>90</v>
-      </c>
+    <row r="18" spans="1:9" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A18" s="43"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="48"/>
       <c r="I18" s="42"/>
     </row>
-    <row r="19" spans="1:9" ht="43.2" x14ac:dyDescent="0.25">
-      <c r="A19" s="52">
-        <v>17</v>
-      </c>
-      <c r="B19" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="49" t="s">
-        <v>91</v>
-      </c>
-      <c r="D19" s="40" t="s">
-        <v>92</v>
-      </c>
-      <c r="E19" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="F19" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="G19" s="45">
-        <v>44782</v>
-      </c>
-      <c r="H19" s="48" t="s">
-        <v>93</v>
-      </c>
+    <row r="19" spans="1:9" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A19" s="52"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="45"/>
+      <c r="H19" s="48"/>
       <c r="I19" s="42"/>
     </row>
-    <row r="20" spans="1:9" ht="43.2" x14ac:dyDescent="0.25">
-      <c r="A20" s="43">
-        <v>18</v>
-      </c>
-      <c r="B20" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" s="49" t="s">
-        <v>94</v>
-      </c>
-      <c r="D20" s="40" t="s">
-        <v>92</v>
-      </c>
-      <c r="E20" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="F20" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="G20" s="47">
-        <v>44785</v>
-      </c>
-      <c r="H20" s="48" t="s">
-        <v>95</v>
-      </c>
+    <row r="20" spans="1:9" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A20" s="43"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="47"/>
+      <c r="H20" s="48"/>
       <c r="I20" s="42"/>
     </row>
-    <row r="21" spans="1:9" ht="43.2" x14ac:dyDescent="0.25">
-      <c r="A21" s="52">
-        <v>19</v>
-      </c>
-      <c r="B21" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21" s="49" t="s">
-        <v>96</v>
-      </c>
-      <c r="D21" s="40" t="s">
-        <v>92</v>
-      </c>
-      <c r="E21" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="F21" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="G21" s="47">
-        <v>44785</v>
-      </c>
-      <c r="H21" s="48" t="s">
-        <v>97</v>
-      </c>
+    <row r="21" spans="1:9" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A21" s="52"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="48"/>
       <c r="I21" s="42"/>
     </row>
-    <row r="22" spans="1:9" ht="43.2" x14ac:dyDescent="0.25">
-      <c r="A22" s="43">
-        <v>20</v>
-      </c>
-      <c r="B22" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" s="49" t="s">
-        <v>98</v>
-      </c>
-      <c r="D22" s="40" t="s">
-        <v>92</v>
-      </c>
-      <c r="E22" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="F22" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="G22" s="45">
-        <v>44785</v>
-      </c>
-      <c r="H22" s="48" t="s">
-        <v>99</v>
-      </c>
+    <row r="22" spans="1:9" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A22" s="43"/>
+      <c r="B22" s="38"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="45"/>
+      <c r="H22" s="48"/>
       <c r="I22" s="42"/>
     </row>
   </sheetData>
@@ -2647,29 +2204,9 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="A1" location="Cover!A1" display="Source Change Log" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="H14" r:id="rId1" xr:uid="{17CE4685-A379-4B6B-B336-CAB58D5D12FF}"/>
-    <hyperlink ref="H3" r:id="rId2" xr:uid="{066ED001-6D67-4608-A3E1-48D8EDB1354D}"/>
-    <hyperlink ref="H4" r:id="rId3" xr:uid="{B18E709D-4156-447B-A5A5-21F6236DC3BE}"/>
-    <hyperlink ref="H5" r:id="rId4" xr:uid="{3C8B6C07-596E-4366-B5E7-CCBF736A24CB}"/>
-    <hyperlink ref="H6" r:id="rId5" xr:uid="{B8F78017-8728-4E1B-A8A0-22F31171C1EF}"/>
-    <hyperlink ref="H7" r:id="rId6" xr:uid="{F8408479-CF45-4831-8728-8C3F2B226A02}"/>
-    <hyperlink ref="H8" r:id="rId7" xr:uid="{476F8404-3A3F-4C1D-99AE-859F3193BD40}"/>
-    <hyperlink ref="H9" r:id="rId8" xr:uid="{6798CB6F-5779-434C-BE24-C24870E1466A}"/>
-    <hyperlink ref="H10" r:id="rId9" xr:uid="{8E57704B-6C1D-4FF2-8367-D57A0C56E0D8}"/>
-    <hyperlink ref="H11" r:id="rId10" xr:uid="{0095B4A0-CC80-4900-ADB9-FF9708300E7C}"/>
-    <hyperlink ref="H12" r:id="rId11" xr:uid="{2A45F263-5833-481E-80DA-F5DAF817E083}"/>
-    <hyperlink ref="H13" r:id="rId12" xr:uid="{A70753B8-C6A5-442D-A082-E39198F6C21C}"/>
-    <hyperlink ref="H15" r:id="rId13" xr:uid="{FF2E85E9-3FA1-48F9-A2ED-1E85812164B3}"/>
-    <hyperlink ref="H16" r:id="rId14" xr:uid="{CCD7D593-6429-44BD-A1D2-CAEEBB7C64CC}"/>
-    <hyperlink ref="H17" r:id="rId15" xr:uid="{704EB59A-CD47-46DF-9780-5547B1F2D702}"/>
-    <hyperlink ref="H18" r:id="rId16" xr:uid="{EADFDD82-7983-48C9-ADCF-55BB680458AD}"/>
-    <hyperlink ref="H19" r:id="rId17" xr:uid="{64DCC7CA-6C5D-4129-A2B0-C2FDE85B8FAB}"/>
-    <hyperlink ref="H20" r:id="rId18" xr:uid="{92231DEB-8247-46E3-A63A-E4C1C8ACD278}"/>
-    <hyperlink ref="H21" r:id="rId19" xr:uid="{5C31297E-44D6-4625-97F6-BE3594A9A657}"/>
-    <hyperlink ref="H22" r:id="rId20" xr:uid="{06970A8B-49F1-4821-BB98-67B3D298D8ED}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId21"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2697,38 +2234,38 @@
   <sheetData>
     <row r="1" spans="1:9" ht="22.8" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="23"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B2" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="F2" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="G2" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="H2" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="I2" s="18" t="s">
         <v>50</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="I2" s="18" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2788,38 +2325,38 @@
   <sheetData>
     <row r="1" spans="1:9" ht="22.8" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="23"/>
     </row>
     <row r="2" spans="1:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B2" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="F2" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="G2" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="H2" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="I2" s="18" t="s">
         <v>50</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="I2" s="18" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2872,88 +2409,88 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>100</v>
+        <v>56</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C2" t="s">
-        <v>101</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>102</v>
+        <v>58</v>
       </c>
       <c r="C3" t="s">
-        <v>103</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="19" t="s">
-        <v>104</v>
+        <v>60</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="19" t="s">
-        <v>105</v>
+        <v>61</v>
       </c>
       <c r="C5" t="s">
-        <v>106</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="19" t="s">
-        <v>107</v>
+        <v>63</v>
       </c>
       <c r="C6" t="s">
-        <v>83</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="19" t="s">
-        <v>108</v>
+        <v>64</v>
       </c>
       <c r="C7" t="s">
-        <v>92</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="19" t="s">
-        <v>109</v>
+        <v>65</v>
       </c>
       <c r="C8" t="s">
-        <v>110</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="19" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>111</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="19" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -2989,17 +2526,17 @@
   <sheetData>
     <row r="1" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>112</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>113</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>114</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -3008,22 +2545,22 @@
     <row r="5" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:6" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
-        <v>115</v>
+        <v>71</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>116</v>
+        <v>72</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>117</v>
+        <v>73</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>118</v>
+        <v>74</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>119</v>
+        <v>75</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>120</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -3031,13 +2568,13 @@
         <v>44257</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>121</v>
+        <v>77</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>122</v>
+        <v>78</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>123</v>
+        <v>79</v>
       </c>
       <c r="E7" s="14"/>
       <c r="F7" s="14"/>
@@ -3073,12 +2610,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3214,15 +2748,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1BB6136B-6A54-49EB-94C3-1CE33ACD540D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F67BDBB-3D91-45AE-B771-A0EA7A408106}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3246,10 +2784,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F67BDBB-3D91-45AE-B771-A0EA7A408106}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1BB6136B-6A54-49EB-94C3-1CE33ACD540D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>